<commit_message>
Updated the excel-sheet feedprofile
</commit_message>
<xml_diff>
--- a/Amribt_lab.xlsx
+++ b/Amribt_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpeter/Code/Modelica/GitHub/Colab/BPL_CHO_Fedbatch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD4121-8A42-EE47-8963-2D09814C8B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3519EA8C-B073-A84F-8117-A39A26928366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50080" yWindow="-1760" windowWidth="24920" windowHeight="20120" xr2:uid="{372148BB-9BFC-9D43-B43D-7E63A7D56CEA}"/>
+    <workbookView xWindow="-44520" yWindow="-1820" windowWidth="24920" windowHeight="20120" activeTab="1" xr2:uid="{372148BB-9BFC-9D43-B43D-7E63A7D56CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_values" sheetId="1" r:id="rId1"/>
@@ -744,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D710195A-1C63-774B-AE6C-FE6E3B7AE8E9}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E80FCD-33D1-FD42-97CB-B235D113414F}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,6 +954,9 @@
         <v>89</v>
       </c>
       <c r="C6" s="6">
+        <v>1001</v>
+      </c>
+      <c r="D6" s="6">
         <v>50</v>
       </c>
     </row>
@@ -965,6 +968,9 @@
         <v>90</v>
       </c>
       <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -976,6 +982,9 @@
         <v>91</v>
       </c>
       <c r="C8" s="6">
+        <v>1002</v>
+      </c>
+      <c r="D8" s="6">
         <v>64</v>
       </c>
     </row>
@@ -987,6 +996,9 @@
         <v>92</v>
       </c>
       <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
         <v>2E-3</v>
       </c>
     </row>
@@ -998,6 +1010,9 @@
         <v>93</v>
       </c>
       <c r="C10" s="6">
+        <v>1003</v>
+      </c>
+      <c r="D10" s="6">
         <v>78</v>
       </c>
     </row>
@@ -1009,6 +1024,9 @@
         <v>94</v>
       </c>
       <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -1020,6 +1038,9 @@
         <v>95</v>
       </c>
       <c r="C12" s="6">
+        <v>1004</v>
+      </c>
+      <c r="D12" s="6">
         <v>92</v>
       </c>
     </row>
@@ -1031,6 +1052,9 @@
         <v>96</v>
       </c>
       <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -1042,6 +1066,9 @@
         <v>97</v>
       </c>
       <c r="C14" s="6">
+        <v>1005</v>
+      </c>
+      <c r="D14" s="6">
         <v>106</v>
       </c>
     </row>
@@ -1053,6 +1080,9 @@
         <v>98</v>
       </c>
       <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -1064,10 +1094,13 @@
         <v>99</v>
       </c>
       <c r="C16" s="6">
+        <v>1006</v>
+      </c>
+      <c r="D16" s="6">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>58</v>
       </c>
@@ -1075,6 +1108,9 @@
         <v>100</v>
       </c>
       <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
         <v>1.2E-2</v>
       </c>
     </row>

</xml_diff>